<commit_message>
Add "EQ" "blank" comparator
</commit_message>
<xml_diff>
--- a/inst/extdata/exampleARS_3.xlsx
+++ b/inst/extdata/exampleARS_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clymb-my.sharepoint.com/personal/mbosman_clymb_onmicrosoft_com/Documents/Documents/siera/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_E75126E222C69DF390F1E656046825349E65D396" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0CF0427-B259-44CA-98B5-785F3F7BBCF9}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_E75126E222C69DF390F1E656046825349E65D396" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D637438C-FC4A-4803-9396-90597DB66C00}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="20" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2025,7 +2025,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2033,7 +2033,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4958,7 +4957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -9904,7 +9903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4:M13"/>
     </sheetView>
   </sheetViews>
@@ -11020,13 +11019,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="78.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -11053,7 +11055,7 @@
       <c r="C2" t="s">
         <v>576</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" t="s">
         <v>613</v>
       </c>
     </row>
@@ -11067,7 +11069,7 @@
       <c r="C3" t="s">
         <v>576</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>614</v>
       </c>
     </row>
@@ -11081,7 +11083,7 @@
       <c r="C4" t="s">
         <v>576</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>615</v>
       </c>
     </row>
@@ -11094,7 +11096,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -11579,7 +11581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -11750,7 +11754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD96"/>
     </sheetView>
   </sheetViews>

</xml_diff>